<commit_message>
Uygulama güncellendi: test ekranı ve panel düzeni
</commit_message>
<xml_diff>
--- a/assets/db/electronic_components_db.xlsx
+++ b/assets/db/electronic_components_db.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,27 +489,22 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>test_script_id</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>hfe</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>speed</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>test_script_id</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>datasheet_url</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>manufacturer</t>
         </is>
       </c>
     </row>
@@ -552,21 +547,20 @@
         <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0175</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0</v>
-      </c>
-      <c r="M2" t="inlineStr">
+        <v>0.017</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>TEST_MOSFET_N</t>
         </is>
       </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Düşük dirençli, genel amaçlı güç MOSFET'i.</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -609,89 +603,87 @@
       <c r="J3" t="n">
         <v>0.008</v>
       </c>
-      <c r="K3" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="inlineStr">
+      <c r="K3" t="inlineStr">
         <is>
           <t>TEST_MOSFET_N</t>
         </is>
       </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Çok yüksek akım kapasiteli, inverterler için ideal MOSFET.</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BC547</t>
+          <t>IRF540N</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BJT</t>
+          <t>MOSFET</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>NPN</t>
+          <t>N-Channel</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>TO-92</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>CBE</t>
+          <t>GDS</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>45</v>
+        <v>100</v>
       </c>
       <c r="G4" t="n">
-        <v>0.1</v>
+        <v>33</v>
       </c>
       <c r="H4" t="n">
-        <v>0.5</v>
+        <v>130</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6</v>
+        <v>4</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>110</v>
-      </c>
-      <c r="L4" t="n">
-        <v>300</v>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>TEST_BJT_NPN</t>
-        </is>
-      </c>
+        <v>0.044</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>TEST_MOSFET_N</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>100V dayanımlı orta güç MOSFET'i.</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TIP31C</t>
+          <t>IRF640</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BJT</t>
+          <t>MOSFET</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NPN</t>
+          <t>N-Channel</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -701,162 +693,159 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>GDS</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="H5" t="n">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="I5" t="n">
-        <v>1.2</v>
+        <v>4</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>25</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>TEST_BJT_NPN</t>
-        </is>
-      </c>
+        <v>0.15</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>TEST_MOSFET_N</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>200V Yüksek voltaj anahtarlama MOSFET'i.</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>UF4007</t>
+          <t>IRF740</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DIODE</t>
+          <t>MOSFET</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Fast Rec</t>
+          <t>N-Channel</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>DO-41</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>AK</t>
+          <t>GDS</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>1000</v>
+        <v>400</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>75</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>TEST_DIODE</t>
-        </is>
-      </c>
+        <v>0.55</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>TEST_MOSFET_N</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>400V SMPS ve sürücü devreleri için MOSFET.</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1N4007</t>
+          <t>IRF840</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DIODE</t>
+          <t>MOSFET</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Standard</t>
+          <t>N-Channel</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DO-41</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>AK</t>
+          <t>GDS</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="I7" t="n">
-        <v>1.1</v>
+        <v>4</v>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>TEST_DIODE</t>
-        </is>
-      </c>
+        <v>0.85</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>TEST_MOSFET_N</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>500V Yüksek voltajlı uygulamalar için.</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>L7805</t>
+          <t>IRF9540</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>REGULATOR</t>
+          <t>MOSFET</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Linear</t>
+          <t>P-Channel</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -866,147 +855,1524 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>IGO</t>
+          <t>GDS</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>35</v>
+        <v>-100</v>
       </c>
       <c r="G8" t="n">
-        <v>1.5</v>
+        <v>-23</v>
       </c>
       <c r="H8" t="n">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="I8" t="n">
-        <v>5</v>
+        <v>-4</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>TEST_REGULATOR</t>
-        </is>
-      </c>
+        <v>0.117</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>TEST_MOSFET_P</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>P-Kanal Güç MOSFET'i (High-Side Switching).</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NE555</t>
+          <t>2N7000</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>IC</t>
+          <t>MOSFET</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Timer</t>
+          <t>N-Channel</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>DIP-8</t>
+          <t>TO-92</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>SGD</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="G9" t="n">
         <v>0.2</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="I9" t="n">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>TEST_IC</t>
-        </is>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>TEST_MOSFET_N</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Küçük sinyal anahtarlama MOSFET'i (Arduino uyumlu).</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LM358</t>
+          <t>BC547</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>IC</t>
+          <t>BJT</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>OpAmp</t>
+          <t>NPN</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>DIP-8</t>
+          <t>TO-92</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>CBE</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="G10" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H10" t="n">
         <v>0.5</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Genel amaçlı, düşük gürültülü NPN transistör.</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>110</v>
+      </c>
+      <c r="N10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BC557</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>PNP</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>TO-92</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>CBE</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>-45</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>TEST_BJT_PNP</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>BC547'nin PNP tamamlayıcısı.</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>110</v>
+      </c>
+      <c r="N11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2N2222</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>NPN</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>TO-92</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>EBC</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>40</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Yüksek hızlı anahtarlama transistörü.</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>100</v>
+      </c>
+      <c r="N12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TIP31C</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>NPN</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>TO-220</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>100</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>40</v>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Orta güç NPN transistörü (Ses ve DC motor).</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>25</v>
+      </c>
+      <c r="N13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>TIP32C</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>PNP</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>TO-220</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>-100</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>40</v>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>TEST_BJT_PNP</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>TIP31C'nin PNP tamamlayıcısı.</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>25</v>
+      </c>
+      <c r="N14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TIP120</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>NPN Darlington</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>TO-220</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>60</v>
+      </c>
+      <c r="G15" t="n">
+        <v>5</v>
+      </c>
+      <c r="H15" t="n">
+        <v>65</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Darlington Transistör. Çok düşük akımla yüksek yükleri sürer.</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>1000</v>
+      </c>
+      <c r="N15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>BD139</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>NPN</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>TO-126</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>ECB</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>80</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>12</v>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Sürücü devreleri için orta güç transistörü.</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>63</v>
+      </c>
+      <c r="N16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2N3055</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>NPN Power</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>TO-3</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>BCE</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>60</v>
+      </c>
+      <c r="G17" t="n">
+        <v>15</v>
+      </c>
+      <c r="H17" t="n">
+        <v>115</v>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Metal kılıf efsanevi güç transistörü.</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>20</v>
+      </c>
+      <c r="N17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>NE555</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>IC</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Timer</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>DIP-8</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>16</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>TEST_IC</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Hassas zamanlayıcı. Osilatör ve PWM devrelerinin kalbi.</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>LM358</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>IC</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>OpAmp Dual</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>DIP-8</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>32</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>TEST_IC</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Çift kanallı, tek beslemeyle çalışan Op-Amp.</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>LM741</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>IC</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>OpAmp Single</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>DIP-8</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>12345678</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>22</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>TEST_IC</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Klasik tekli Op-Amp. Eğitim amaçlı ideal.</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>LM324</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>IC</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>OpAmp Quad</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>DIP-14</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>1-14</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>32</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>TEST_IC</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Dörtlü LM358 versiyonu.</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ULN2003</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>IC</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Darlington Array</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>DIP-16</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>50</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>TEST_IC</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>7 Kanal Darlington dizisi. Röle ve step motor sürücü.</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>L293D</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>IC</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Motor Driver</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>DIP-16</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>1-16</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>36</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>TEST_IC</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Çift H-Köprüsü Motor Sürücü.</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>PC817</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>IC</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Optocoupler</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>DIP-4</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>AKEC</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>35</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Sinyal izolasyonu için optokuplör.</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>L7805</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>REGULATOR</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>TO-220</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>IGO</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>35</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H25" t="n">
+        <v>15</v>
+      </c>
+      <c r="I25" t="n">
+        <v>5</v>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>TEST_REGULATOR</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Pozitif 5V Sabit Regülatör.</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>L7809</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>REGULATOR</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>TO-220</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>IGO</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>35</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H26" t="n">
+        <v>15</v>
+      </c>
+      <c r="I26" t="n">
+        <v>9</v>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>TEST_REGULATOR</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Pozitif 9V Sabit Regülatör.</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>L7812</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>REGULATOR</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Linear</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>TO-220</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>IGO</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>35</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H27" t="n">
+        <v>15</v>
+      </c>
+      <c r="I27" t="n">
+        <v>12</v>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>TEST_REGULATOR</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Pozitif 12V Sabit Regülatör.</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>LM317</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>REGULATOR</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Adjust</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>TO-220</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>AIO</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>40</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H28" t="n">
+        <v>20</v>
+      </c>
+      <c r="I28" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>TEST_REGULATOR</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Ayarlanabilir Voltaj Regülatörü.</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>AMS1117-3.3</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>REGULATOR</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>LDO</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>SOT-223</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>GOI</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>15</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I29" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>TEST_REGULATOR</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>3.3V LDO Regülatör (SMD).</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1N4007</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>DIODE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>DO-41</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H30" t="n">
         <v>0</v>
       </c>
-      <c r="J10" t="n">
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Genel amaçlı doğrultucu diyot.</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>1N4148</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>DIODE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Switching</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>DO-35</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>100</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H31" t="n">
         <v>0</v>
       </c>
-      <c r="K10" t="n">
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Yüksek hızlı sinyal diyodu.</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>UF4007</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>DIODE</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Fast Rec</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>DO-41</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" t="n">
         <v>0</v>
       </c>
-      <c r="L10" t="n">
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Ultra Hızlı (Fast Recovery) diyot.</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>1N5819</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>DIODE</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Schottky</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>DO-41</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>40</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" t="n">
         <v>0</v>
       </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>TEST_IC</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Düşük voltaj düşümlü Schottky diyot.</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BC846</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>NPN</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>CBE</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>65</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>SMD NPN Transistör.</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>110</v>
+      </c>
+      <c r="N34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>MMBT3904</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>NPN</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>EBC</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>40</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H35" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>2N3904'ün SMD versiyonu.</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>100</v>
+      </c>
+      <c r="N35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>M7</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>DIODE</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>SMA</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1</v>
+      </c>
+      <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>1N4007'nin SMD versiyonu.</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>SS14</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>DIODE</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Schottky</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>SMA</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>40</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>1N5819'un SMD versiyonu.</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1019,7 +2385,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1064,15 +2430,100 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>1B</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BC847</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1AM</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MMBT3904</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MMBT3906</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>J3Y</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>S8050</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>M7</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1N4007</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>M7</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SMA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>SS14</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>SS14</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>SMA</t>
         </is>
@@ -1089,7 +2540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1124,60 +2575,156 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SOT-23</t>
+          <t>TO-92</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>assets/packages/sot-23.png</t>
+          <t>assets/packages/to-92.png</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TO-92</t>
+          <t>TO-126</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>assets/packages/to-92.png</t>
+          <t>assets/packages/to-220.png</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DO-41</t>
+          <t>TO-3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>assets/packages/do-41.png</t>
+          <t>assets/packages/to-3.png</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SMA</t>
+          <t>DO-41</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>assets/packages/sma.png</t>
+          <t>assets/packages/do-41.png</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>DO-35</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>assets/packages/do-41.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>DO-201</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>assets/packages/do-41.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>assets/packages/sot-23.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SOT-223</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>assets/packages/sot-223.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SMA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>assets/packages/sma.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>DIP-8</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>assets/packages/dip-8.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>DIP-14</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>assets/packages/dip-14.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>DIP-16</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>assets/packages/dip-16.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>DIP-4</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>assets/packages/dip-4.png</t>
         </is>
       </c>
     </row>
@@ -1192,7 +2739,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1227,7 +2774,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TEST_BJT_NPN</t>
+          <t>TEST_MOSFET_P</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1239,7 +2786,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TEST_DIODE</t>
+          <t>TEST_BJT_NPN</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1251,7 +2798,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TEST_REGULATOR</t>
+          <t>TEST_BJT_PNP</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1263,10 +2810,34 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TEST_REGULATOR</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>TEST_IC</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>{}</t>
         </is>

</xml_diff>

<commit_message>
Topluluk özelliği güncellendi - Firebase Storage ve Firestore entegrasyonu tamamlandı
</commit_message>
<xml_diff>
--- a/assets/db/electronic_components_db.xlsx
+++ b/assets/db/electronic_components_db.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,10 +499,15 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>pin_names</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
           <t>hfe</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>speed</t>
         </is>
@@ -556,11 +561,16 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Düşük dirençli, genel amaçlı güç MOSFET'i.</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr"/>
+          <t>Standart N-Kanal Güç MOSFET'i. Motor sürücü ve güç kaynaklarında yaygın.</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>GATE,DRAIN,SOURCE</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -610,11 +620,16 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Çok yüksek akım kapasiteli, inverterler için ideal MOSFET.</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr"/>
+          <t>Çok düşük iç dirençli, yüksek akım MOSFET'i. İnverterler için ideal.</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>GATE,DRAIN,SOURCE</t>
+        </is>
+      </c>
       <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -664,11 +679,16 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>100V dayanımlı orta güç MOSFET'i.</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
+          <t>100V Dayanımlı genel amaçlı güç MOSFET'i.</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>GATE,DRAIN,SOURCE</t>
+        </is>
+      </c>
       <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -718,11 +738,16 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>200V Yüksek voltaj anahtarlama MOSFET'i.</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
+          <t>200V Yüksek voltaj anahtarlama elemanı.</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>GATE,DRAIN,SOURCE</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -772,11 +797,16 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>400V SMPS ve sürücü devreleri için MOSFET.</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr"/>
+          <t>400V SMPS ve sürücü devreleri için.</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>GATE,DRAIN,SOURCE</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -826,11 +856,16 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>500V Yüksek voltajlı uygulamalar için.</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr"/>
+          <t>500V Yüksek voltaj uygulamaları.</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>GATE,DRAIN,SOURCE</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -880,11 +915,16 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>P-Kanal Güç MOSFET'i (High-Side Switching).</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr"/>
+          <t>P-Kanal Güç MOSFET'i (High-Side Anahtarlama).</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>GATE,DRAIN,SOURCE</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -934,26 +974,31 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Küçük sinyal anahtarlama MOSFET'i (Arduino uyumlu).</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr"/>
+          <t>Küçük sinyal, lojik seviye MOSFET. Arduino ile sürülebilir.</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>SOURCE,GATE,DRAIN</t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BC547</t>
+          <t>BS170</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BJT</t>
+          <t>MOSFET</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>NPN</t>
+          <t>N-Channel</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -963,39 +1008,46 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CBE</t>
+          <t>DGS</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G10" t="n">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H10" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
+        <v>0.8</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>5</v>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>TEST_BJT_NPN</t>
+          <t>TEST_MOSFET_N</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Genel amaçlı, düşük gürültülü NPN transistör.</t>
-        </is>
-      </c>
-      <c r="M10" t="n">
-        <v>110</v>
+          <t>2N7000 benzeri ama bacak dizilimi farklı (DGS).</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>DRAIN,GATE,SOURCE</t>
+        </is>
       </c>
       <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BC557</t>
+          <t>BC547</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1005,7 +1057,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PNP</t>
+          <t>NPN</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1019,10 +1071,10 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>-45</v>
+        <v>45</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.1</v>
+        <v>0.1</v>
       </c>
       <c r="H11" t="n">
         <v>0.5</v>
@@ -1031,23 +1083,28 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr">
         <is>
-          <t>TEST_BJT_PNP</t>
+          <t>TEST_BJT_NPN</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>BC547'nin PNP tamamlayıcısı.</t>
-        </is>
-      </c>
-      <c r="M11" t="n">
+          <t>Genel amaçlı, düşük gürültülü NPN.</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>COLL,BASE,EMIT</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
         <v>110</v>
       </c>
-      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2N2222</t>
+          <t>BC557</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1057,7 +1114,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>NPN</t>
+          <t>PNP</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -1067,14 +1124,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>EBC</t>
+          <t>CBE</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>40</v>
+        <v>-45</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8</v>
+        <v>-0.1</v>
       </c>
       <c r="H12" t="n">
         <v>0.5</v>
@@ -1083,23 +1140,28 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr">
         <is>
-          <t>TEST_BJT_NPN</t>
+          <t>TEST_BJT_PNP</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Yüksek hızlı anahtarlama transistörü.</t>
-        </is>
-      </c>
-      <c r="M12" t="n">
-        <v>100</v>
-      </c>
-      <c r="N12" t="inlineStr"/>
+          <t>Genel amaçlı PNP transistör.</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>COLL,BASE,EMIT</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>110</v>
+      </c>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>TIP31C</t>
+          <t>2N2222</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1114,22 +1176,22 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>TO-220</t>
+          <t>TO-92</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>EBC</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="G13" t="n">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="H13" t="n">
-        <v>40</v>
+        <v>0.5</v>
       </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
@@ -1140,18 +1202,23 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Orta güç NPN transistörü (Ses ve DC motor).</t>
-        </is>
-      </c>
-      <c r="M13" t="n">
-        <v>25</v>
-      </c>
-      <c r="N13" t="inlineStr"/>
+          <t>Yüksek hızlı anahtarlama ve yükseltme.</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>EMIT,BASE,COLL</t>
+        </is>
+      </c>
+      <c r="N13" t="n">
+        <v>100</v>
+      </c>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TIP32C</t>
+          <t>2N3904</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1161,49 +1228,54 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>PNP</t>
+          <t>NPN</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>TO-220</t>
+          <t>TO-92</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>EBC</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>-100</v>
+        <v>40</v>
       </c>
       <c r="G14" t="n">
-        <v>-3</v>
+        <v>0.2</v>
       </c>
       <c r="H14" t="n">
-        <v>40</v>
+        <v>0.6</v>
       </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr">
         <is>
-          <t>TEST_BJT_PNP</t>
+          <t>TEST_BJT_NPN</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>TIP31C'nin PNP tamamlayıcısı.</t>
-        </is>
-      </c>
-      <c r="M14" t="n">
-        <v>25</v>
-      </c>
-      <c r="N14" t="inlineStr"/>
+          <t>Genel amaçlı NPN.</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>EMIT,BASE,COLL</t>
+        </is>
+      </c>
+      <c r="N14" t="n">
+        <v>100</v>
+      </c>
+      <c r="O14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TIP120</t>
+          <t>BD139</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1213,27 +1285,27 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NPN Darlington</t>
+          <t>NPN</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>TO-220</t>
+          <t>TO-126</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>ECB</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G15" t="n">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="H15" t="n">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
@@ -1244,18 +1316,23 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Darlington Transistör. Çok düşük akımla yüksek yükleri sürer.</t>
-        </is>
-      </c>
-      <c r="M15" t="n">
-        <v>1000</v>
-      </c>
-      <c r="N15" t="inlineStr"/>
+          <t>Orta güç NPN. Ses sürücü devrelerinde sıkça kullanılır.</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>EMIT,COLL,BASE</t>
+        </is>
+      </c>
+      <c r="N15" t="n">
+        <v>63</v>
+      </c>
+      <c r="O15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BD139</t>
+          <t>BD140</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1265,7 +1342,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>NPN</t>
+          <t>PNP</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1279,10 +1356,10 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>80</v>
+        <v>-80</v>
       </c>
       <c r="G16" t="n">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="H16" t="n">
         <v>12</v>
@@ -1291,23 +1368,28 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr">
         <is>
-          <t>TEST_BJT_NPN</t>
+          <t>TEST_BJT_PNP</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Sürücü devreleri için orta güç transistörü.</t>
-        </is>
-      </c>
-      <c r="M16" t="n">
+          <t>BD139'un PNP eşleniği.</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>EMIT,COLL,BASE</t>
+        </is>
+      </c>
+      <c r="N16" t="n">
         <v>63</v>
       </c>
-      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2N3055</t>
+          <t>TIP31C</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1317,12 +1399,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>NPN Power</t>
+          <t>NPN</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>TO-3</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1331,13 +1413,13 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="G17" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H17" t="n">
-        <v>115</v>
+        <v>40</v>
       </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
@@ -1348,168 +1430,194 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Metal kılıf efsanevi güç transistörü.</t>
-        </is>
-      </c>
-      <c r="M17" t="n">
-        <v>20</v>
-      </c>
-      <c r="N17" t="inlineStr"/>
+          <t>Güç NPN Transistörü.</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>BASE,COLL,EMIT</t>
+        </is>
+      </c>
+      <c r="N17" t="n">
+        <v>25</v>
+      </c>
+      <c r="O17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>NE555</t>
+          <t>TIP32C</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>IC</t>
+          <t>BJT</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Timer</t>
+          <t>PNP</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>DIP-8</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>BCE</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>16</v>
+        <v>-100</v>
       </c>
       <c r="G18" t="n">
-        <v>0.2</v>
+        <v>-3</v>
       </c>
       <c r="H18" t="n">
-        <v>0.6</v>
+        <v>40</v>
       </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr">
         <is>
-          <t>TEST_IC</t>
+          <t>TEST_BJT_PNP</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Hassas zamanlayıcı. Osilatör ve PWM devrelerinin kalbi.</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr"/>
-      <c r="N18" t="inlineStr"/>
+          <t>Güç PNP Transistörü.</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>BASE,COLL,EMIT</t>
+        </is>
+      </c>
+      <c r="N18" t="n">
+        <v>25</v>
+      </c>
+      <c r="O18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LM358</t>
+          <t>TIP120</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>IC</t>
+          <t>BJT</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>OpAmp Dual</t>
+          <t>NPN Darlington</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>DIP-8</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>BCE</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="G19" t="n">
-        <v>0.02</v>
+        <v>5</v>
       </c>
       <c r="H19" t="n">
-        <v>0.5</v>
+        <v>65</v>
       </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr">
         <is>
-          <t>TEST_IC</t>
+          <t>TEST_BJT_NPN</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Çift kanallı, tek beslemeyle çalışan Op-Amp.</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr"/>
-      <c r="N19" t="inlineStr"/>
+          <t>Darlington NPN. Çok yüksek kazançlı.</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>BASE,COLL,EMIT</t>
+        </is>
+      </c>
+      <c r="N19" t="n">
+        <v>1000</v>
+      </c>
+      <c r="O19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>LM741</t>
+          <t>2N3055</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>IC</t>
+          <t>BJT</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>OpAmp Single</t>
+          <t>NPN Power</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>DIP-8</t>
+          <t>TO-3</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>BCE</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="G20" t="n">
-        <v>0.002</v>
+        <v>15</v>
       </c>
       <c r="H20" t="n">
-        <v>0.5</v>
+        <v>115</v>
       </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr">
         <is>
-          <t>TEST_IC</t>
+          <t>TEST_BJT_NPN</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Klasik tekli Op-Amp. Eğitim amaçlı ideal.</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr"/>
-      <c r="N20" t="inlineStr"/>
+          <t>Efsanevi metal kılıf güç transistörü.</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>BASE,COLL,EMIT</t>
+        </is>
+      </c>
+      <c r="N20" t="n">
+        <v>20</v>
+      </c>
+      <c r="O20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>LM324</t>
+          <t>NE555</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1519,27 +1627,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>OpAmp Quad</t>
+          <t>Timer</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>DIP-14</t>
+          <t>DIP-8</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1-14</t>
+          <t>1-8</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G21" t="n">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
       <c r="H21" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
@@ -1550,16 +1658,21 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Dörtlü LM358 versiyonu.</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr"/>
+          <t>Hassas zamanlayıcı. Osilatör, PWM ve Timer devrelerinin kalbi.</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>GND,TRIG,OUT,RST,CTRL,THR,DIS,VCC</t>
+        </is>
+      </c>
       <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ULN2003</t>
+          <t>LM358</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1569,27 +1682,27 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Darlington Array</t>
+          <t>OpAmp Dual</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>DIP-16</t>
+          <t>DIP-8</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1-16</t>
+          <t>1-8</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="G22" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H22" t="n">
         <v>0.5</v>
-      </c>
-      <c r="H22" t="n">
-        <v>1</v>
       </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
@@ -1600,16 +1713,21 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>7 Kanal Darlington dizisi. Röle ve step motor sürücü.</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr"/>
+          <t>Çift kanallı, tek beslemeyle çalışabilen genel amaçlı Op-Amp.</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>OUT A,IN- A,IN+ A,GND,IN+ B,IN- B,OUT B,VCC</t>
+        </is>
+      </c>
       <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>L293D</t>
+          <t>LM741</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1619,27 +1737,27 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Motor Driver</t>
+          <t>OpAmp Single</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>DIP-16</t>
+          <t>DIP-8</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>1-16</t>
+          <t>1-8</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G23" t="n">
-        <v>0.6</v>
+        <v>0.002</v>
       </c>
       <c r="H23" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
@@ -1650,16 +1768,21 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Çift H-Köprüsü Motor Sürücü.</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr"/>
+          <t>Klasik tekli Op-Amp. Eğitim ve temel uygulamalar için.</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>OFF,IN-,IN+,V-,OFF,OUT,V+,NC</t>
+        </is>
+      </c>
       <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>PC817</t>
+          <t>TL072</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1669,255 +1792,272 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Optocoupler</t>
+          <t>JFET OpAmp</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>DIP-4</t>
+          <t>DIP-8</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>AKEC</t>
+          <t>1-8</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G24" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="H24" t="n">
-        <v>0.15</v>
+        <v>0.6</v>
       </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr">
         <is>
-          <t>TEST_DIODE</t>
+          <t>TEST_IC</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Sinyal izolasyonu için optokuplör.</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr"/>
+          <t>Düşük gürültülü JFET girişli Op-Amp. Ses devreleri için ideal.</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>OUT A,IN- A,IN+ A,V-,IN+ B,IN- B,OUT B,V+</t>
+        </is>
+      </c>
       <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>L7805</t>
+          <t>ULN2003</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>REGULATOR</t>
+          <t>IC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Linear</t>
+          <t>Darlington</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>TO-220</t>
+          <t>DIP-16</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>IGO</t>
+          <t>1-16</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="G25" t="n">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="H25" t="n">
-        <v>15</v>
-      </c>
-      <c r="I25" t="n">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr">
         <is>
-          <t>TEST_REGULATOR</t>
+          <t>TEST_IC</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pozitif 5V Sabit Regülatör.</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr"/>
+          <t>7 Kanal Darlington dizisi. Röle ve step motor sürmek için kullanılır.</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>IN1,IN2,IN3,IN4,IN5,IN6,IN7,GND,COM,OUT7,OUT6,OUT5,OUT4,OUT3,OUT2,OUT1</t>
+        </is>
+      </c>
       <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>L7809</t>
+          <t>L293D</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>REGULATOR</t>
+          <t>IC</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Linear</t>
+          <t>Motor Driver</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>TO-220</t>
+          <t>DIP-16</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>IGO</t>
+          <t>1-16</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G26" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="H26" t="n">
         <v>1.5</v>
       </c>
-      <c r="H26" t="n">
-        <v>15</v>
-      </c>
-      <c r="I26" t="n">
-        <v>9</v>
-      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr">
         <is>
-          <t>TEST_REGULATOR</t>
+          <t>TEST_IC</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pozitif 9V Sabit Regülatör.</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr"/>
+          <t>Çift H-Köprüsü Motor Sürücü. DC motorları ileri-geri sürebilir.</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>EN1,IN1,OUT1,GND,GND,OUT2,IN2,VCC2,EN2,IN3,OUT3,GND,GND,OUT4,IN4,VCC1</t>
+        </is>
+      </c>
       <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>L7812</t>
+          <t>CD4017</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>REGULATOR</t>
+          <t>IC</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Linear</t>
+          <t>Counter</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>TO-220</t>
+          <t>DIP-16</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>IGO</t>
+          <t>1-16</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="G27" t="n">
-        <v>1.5</v>
+        <v>0.01</v>
       </c>
       <c r="H27" t="n">
-        <v>15</v>
-      </c>
-      <c r="I27" t="n">
-        <v>12</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr">
         <is>
-          <t>TEST_REGULATOR</t>
+          <t>TEST_IC</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pozitif 12V Sabit Regülatör.</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr"/>
+          <t>Onlu sayıcı (Decade Counter). Yürüyen ışık devrelerinde popülerdir.</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>5,1,0,2,6,7,3,GND,8,4,9,CARRY,EN,CLK,RST,VCC</t>
+        </is>
+      </c>
       <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>LM317</t>
+          <t>PC817</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>REGULATOR</t>
+          <t>IC</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Adjust</t>
+          <t>Optocoupler</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>TO-220</t>
+          <t>DIP-4</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>AIO</t>
+          <t>AKEC</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G28" t="n">
-        <v>1.5</v>
+        <v>0.05</v>
       </c>
       <c r="H28" t="n">
-        <v>20</v>
-      </c>
-      <c r="I28" t="n">
-        <v>1.25</v>
-      </c>
+        <v>0.15</v>
+      </c>
+      <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr">
         <is>
-          <t>TEST_REGULATOR</t>
+          <t>TEST_DIODE</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Ayarlanabilir Voltaj Regülatörü.</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr"/>
+          <t>4 Pinli Optokuplör. Sinyal izolasyonu sağlar.</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>ANODE,CATHODE,EMITTER,COLLECTOR</t>
+        </is>
+      </c>
       <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>AMS1117-3.3</t>
+          <t>L7805</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1927,30 +2067,30 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>LDO</t>
+          <t>Linear</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>SOT-223</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>GOI</t>
+          <t>IGO</t>
         </is>
       </c>
       <c r="F29" t="n">
+        <v>35</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="H29" t="n">
         <v>15</v>
       </c>
-      <c r="G29" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="H29" t="n">
-        <v>1</v>
-      </c>
       <c r="I29" t="n">
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr">
@@ -1960,324 +2100,361 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>3.3V LDO Regülatör (SMD).</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr"/>
+          <t>Pozitif 5V Sabit Regülatör.</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>INPUT,GND,OUTPUT</t>
+        </is>
+      </c>
       <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1N4007</t>
+          <t>L7809</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>DIODE</t>
+          <t>REGULATOR</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Standard</t>
+          <t>Linear</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>DO-41</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>AK</t>
+          <t>IGO</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1000</v>
+        <v>35</v>
       </c>
       <c r="G30" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
-      </c>
-      <c r="I30" t="inlineStr"/>
+        <v>15</v>
+      </c>
+      <c r="I30" t="n">
+        <v>9</v>
+      </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr">
         <is>
-          <t>TEST_DIODE</t>
+          <t>TEST_REGULATOR</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Genel amaçlı doğrultucu diyot.</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr"/>
+          <t>Pozitif 9V Sabit Regülatör.</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>INPUT,GND,OUTPUT</t>
+        </is>
+      </c>
       <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1N4148</t>
+          <t>L7812</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DIODE</t>
+          <t>REGULATOR</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Switching</t>
+          <t>Linear</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>DO-35</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>AK</t>
+          <t>IGO</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="G31" t="n">
-        <v>0.2</v>
+        <v>1.5</v>
       </c>
       <c r="H31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" t="inlineStr"/>
+        <v>15</v>
+      </c>
+      <c r="I31" t="n">
+        <v>12</v>
+      </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr">
         <is>
-          <t>TEST_DIODE</t>
+          <t>TEST_REGULATOR</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Yüksek hızlı sinyal diyodu.</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr"/>
-      <c r="N31" t="n">
-        <v>4</v>
-      </c>
+          <t>Pozitif 12V Sabit Regülatör.</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>INPUT,GND,OUTPUT</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>UF4007</t>
+          <t>L7905</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>DIODE</t>
+          <t>REGULATOR</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Fast Rec</t>
+          <t>Negative</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>DO-41</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>AK</t>
+          <t>GIO</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>1000</v>
+        <v>-35</v>
       </c>
       <c r="G32" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H32" t="n">
-        <v>0</v>
-      </c>
-      <c r="I32" t="inlineStr"/>
+        <v>15</v>
+      </c>
+      <c r="I32" t="n">
+        <v>-5</v>
+      </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr">
         <is>
-          <t>TEST_DIODE</t>
+          <t>TEST_REGULATOR</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Ultra Hızlı (Fast Recovery) diyot.</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr"/>
-      <c r="N32" t="n">
-        <v>75</v>
-      </c>
+          <t>Negatif -5V Sabit Regülatör. (GND-Input-Out).</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>GND,INPUT,OUTPUT</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1N5819</t>
+          <t>LM317</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>DIODE</t>
+          <t>REGULATOR</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Schottky</t>
+          <t>Adjust</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>DO-41</t>
+          <t>TO-220</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>AK</t>
+          <t>AOI</t>
         </is>
       </c>
       <c r="F33" t="n">
         <v>40</v>
       </c>
       <c r="G33" t="n">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="I33" t="n">
+        <v>1.25</v>
+      </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr">
         <is>
-          <t>TEST_DIODE</t>
+          <t>TEST_REGULATOR</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Düşük voltaj düşümlü Schottky diyot.</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr"/>
+          <t>Ayarlanabilir Pozitif Regülatör (1.2V - 37V).</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>ADJ,OUTPUT,INPUT</t>
+        </is>
+      </c>
       <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BC846</t>
+          <t>AMS1117-3.3</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>BJT</t>
+          <t>REGULATOR</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>NPN</t>
+          <t>LDO</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>SOT-23</t>
+          <t>SOT-223</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>CBE</t>
+          <t>GOI</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="G34" t="n">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="H34" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="I34" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="I34" t="n">
+        <v>3.3</v>
+      </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr">
         <is>
-          <t>TEST_BJT_NPN</t>
+          <t>TEST_REGULATOR</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>SMD NPN Transistör.</t>
-        </is>
-      </c>
-      <c r="M34" t="n">
-        <v>110</v>
+          <t>3.3V LDO Regülatör (SMD).</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>GND,OUTPUT,INPUT</t>
+        </is>
       </c>
       <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MMBT3904</t>
+          <t>1N4007</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>BJT</t>
+          <t>DIODE</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>NPN</t>
+          <t>Standard</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>SOT-23</t>
+          <t>DO-41</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>EBC</t>
+          <t>AK</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>40</v>
+        <v>1000</v>
       </c>
       <c r="G35" t="n">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="H35" t="n">
-        <v>0.35</v>
+        <v>0</v>
       </c>
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr">
         <is>
-          <t>TEST_BJT_NPN</t>
+          <t>TEST_DIODE</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>2N3904'ün SMD versiyonu.</t>
-        </is>
-      </c>
-      <c r="M35" t="n">
-        <v>100</v>
+          <t>Genel amaçlı doğrultucu diyot.</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>ANODE,CATHODE</t>
+        </is>
       </c>
       <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>M7</t>
+          <t>1N4148</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2287,12 +2464,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Standard</t>
+          <t>Switching</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>SMA</t>
+          <t>DO-35</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2301,10 +2478,10 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="G36" t="n">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="H36" t="n">
         <v>0</v>
@@ -2318,16 +2495,23 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>1N4007'nin SMD versiyonu.</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr"/>
+          <t>Yüksek hızlı sinyal diyodu.</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>ANODE,CATHODE</t>
+        </is>
+      </c>
       <c r="N36" t="inlineStr"/>
+      <c r="O36" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>SS14</t>
+          <t>UF4007</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2337,12 +2521,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Schottky</t>
+          <t>Fast Rec</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>SMA</t>
+          <t>DO-41</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2351,7 +2535,7 @@
         </is>
       </c>
       <c r="F37" t="n">
-        <v>40</v>
+        <v>1000</v>
       </c>
       <c r="G37" t="n">
         <v>1</v>
@@ -2368,11 +2552,297 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
+          <t>Ultra Hızlı (Fast Recovery) diyot.</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>ANODE,CATHODE</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>1N5819</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>DIODE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Schottky</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>DO-41</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>40</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Düşük voltaj düşümlü Schottky diyot.</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>ANODE,CATHODE</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>BC846</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>NPN</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>CBE</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>65</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>SMD NPN Transistör.</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>BASE,EMIT,COLL</t>
+        </is>
+      </c>
+      <c r="N39" t="n">
+        <v>110</v>
+      </c>
+      <c r="O39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>MMBT3904</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>BJT</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>NPN</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>SOT-23</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>EBC</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>40</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>TEST_BJT_NPN</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>2N3904'ün SMD versiyonu.</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>BASE,EMIT,COLL</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>100</v>
+      </c>
+      <c r="O40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>M7</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>DIODE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Standard</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>SMA</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>1N4007'nin SMD versiyonu.</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>ANODE,CATHODE</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SS14</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>DIODE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Schottky</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>SMA</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>AK</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>40</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1</v>
+      </c>
+      <c r="H42" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>TEST_DIODE</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
           <t>1N5819'un SMD versiyonu.</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr"/>
-      <c r="N37" t="inlineStr"/>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>ANODE,CATHODE</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2481,29 +2951,29 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>J3Y</t>
+          <t>M7</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>S8050</t>
+          <t>M7</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SOT-23</t>
+          <t>SMA</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>M7</t>
+          <t>SS14</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>M7</t>
+          <t>SS14</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -2515,17 +2985,17 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>SS14</t>
+          <t>J3Y</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SS14</t>
+          <t>S8050</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>SMA</t>
+          <t>SOT-23</t>
         </is>
       </c>
     </row>
@@ -2683,48 +3153,48 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DIP-8</t>
+          <t>DIP-4</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>assets/packages/dip-8.png</t>
+          <t>assets/packages/dip-4.png</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DIP-14</t>
+          <t>DIP-8</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>assets/packages/dip-14.png</t>
+          <t>assets/packages/dip-8.png</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DIP-16</t>
+          <t>DIP-14</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>assets/packages/dip-16.png</t>
+          <t>assets/packages/dip-14.png</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DIP-4</t>
+          <t>DIP-16</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>assets/packages/dip-4.png</t>
+          <t>assets/packages/dip-16.png</t>
         </is>
       </c>
     </row>

</xml_diff>